<commit_message>
add sumfitness termination rule
</commit_message>
<xml_diff>
--- a/doc/LARGE_SCALE/de_results.xlsx
+++ b/doc/LARGE_SCALE/de_results.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="44">
   <si>
     <t xml:space="preserve">DE_NUMBER(CALLS)</t>
   </si>
@@ -140,19 +140,19 @@
     <t xml:space="preserve">Potential22</t>
   </si>
   <si>
+    <t xml:space="preserve">Potential24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potential26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potential28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potential30</t>
+  </si>
+  <si>
     <t xml:space="preserve">x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Potential24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Potential26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Potential28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Potential30</t>
   </si>
 </sst>
 </file>
@@ -286,10 +286,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B57" activeCellId="0" sqref="B57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E75" activeCellId="0" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1145,185 +1145,347 @@
         <v>29</v>
       </c>
       <c r="B47" s="0" t="n">
-        <v>67768</v>
+        <v>70197</v>
       </c>
       <c r="C47" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E47" s="2"/>
-      <c r="G47" s="2"/>
+      <c r="D47" s="0" t="n">
+        <v>69198</v>
+      </c>
+      <c r="E47" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F47" s="0" t="n">
+        <v>69601</v>
+      </c>
+      <c r="G47" s="2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B48" s="0" t="n">
-        <v>96996</v>
+        <v>99498</v>
       </c>
       <c r="C48" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E48" s="2"/>
-      <c r="G48" s="2"/>
+      <c r="D48" s="0" t="n">
+        <v>120738</v>
+      </c>
+      <c r="E48" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F48" s="0" t="n">
+        <v>90970</v>
+      </c>
+      <c r="G48" s="2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B49" s="0" t="n">
-        <v>89510</v>
+        <v>83868</v>
       </c>
       <c r="C49" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E49" s="2"/>
-      <c r="G49" s="2"/>
+      <c r="D49" s="0" t="n">
+        <v>156906</v>
+      </c>
+      <c r="E49" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <v>82523</v>
+      </c>
+      <c r="G49" s="2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B50" s="0" t="n">
-        <v>79998</v>
+        <v>74666</v>
       </c>
       <c r="C50" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E50" s="2"/>
-      <c r="G50" s="2"/>
+      <c r="D50" s="0" t="n">
+        <v>184608</v>
+      </c>
+      <c r="E50" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F50" s="0" t="n">
+        <v>76802</v>
+      </c>
+      <c r="G50" s="2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>100337</v>
+        <v>79700</v>
       </c>
       <c r="C51" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E51" s="2"/>
-      <c r="G51" s="2"/>
+      <c r="D51" s="0" t="n">
+        <v>263207</v>
+      </c>
+      <c r="E51" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F51" s="0" t="n">
+        <v>83314</v>
+      </c>
+      <c r="G51" s="2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B52" s="0" t="n">
-        <v>76942</v>
+        <v>74016</v>
       </c>
       <c r="C52" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E52" s="2"/>
-      <c r="G52" s="2"/>
+      <c r="D52" s="0" t="n">
+        <v>305432</v>
+      </c>
+      <c r="E52" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F52" s="0" t="n">
+        <v>75177</v>
+      </c>
+      <c r="G52" s="2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B53" s="0" t="n">
-        <v>81402</v>
+        <v>76592</v>
       </c>
       <c r="C53" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E53" s="2"/>
-      <c r="G53" s="2"/>
+      <c r="D53" s="0" t="n">
+        <v>282612</v>
+      </c>
+      <c r="E53" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F53" s="0" t="n">
+        <v>78495</v>
+      </c>
+      <c r="G53" s="2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B54" s="0" t="n">
-        <v>85884</v>
+        <v>77966</v>
       </c>
       <c r="C54" s="2" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="E54" s="2"/>
-      <c r="G54" s="2"/>
+        <v>0.6333</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>473906</v>
+      </c>
+      <c r="E54" s="2" t="n">
+        <v>0.9667</v>
+      </c>
+      <c r="F54" s="0" t="n">
+        <v>80099</v>
+      </c>
+      <c r="G54" s="2" t="n">
+        <v>0.6667</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B55" s="0" t="n">
-        <v>87926</v>
+        <v>84475</v>
       </c>
       <c r="C55" s="2" t="n">
-        <v>0.9333</v>
-      </c>
-      <c r="E55" s="2"/>
-      <c r="G55" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>488927</v>
+      </c>
+      <c r="E55" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F55" s="0" t="n">
+        <v>85246</v>
+      </c>
+      <c r="G55" s="2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B56" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="G56" s="2"/>
+      <c r="B56" s="0" t="n">
+        <v>93651</v>
+      </c>
+      <c r="C56" s="2" t="n">
+        <v>0.9333</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>740144</v>
+      </c>
+      <c r="E56" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F56" s="0" t="n">
+        <v>93996</v>
+      </c>
+      <c r="G56" s="2" t="n">
+        <v>0.9333</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="G57" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>92849</v>
+      </c>
+      <c r="C57" s="2" t="n">
+        <v>0.9333</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>342001</v>
+      </c>
+      <c r="E57" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F57" s="0" t="n">
+        <v>92914</v>
+      </c>
+      <c r="G57" s="2" t="n">
+        <v>0.9333</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C58" s="2"/>
-      <c r="E58" s="2"/>
-      <c r="G58" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>103628</v>
+      </c>
+      <c r="C58" s="2" t="n">
+        <v>0.3333</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>2212139</v>
+      </c>
+      <c r="E58" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F58" s="0" t="n">
+        <v>103710</v>
+      </c>
+      <c r="G58" s="2" t="n">
+        <v>0.3333</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="G59" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>105228</v>
+      </c>
+      <c r="C59" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>1444577</v>
+      </c>
+      <c r="E59" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F59" s="0" t="n">
+        <v>105228</v>
+      </c>
+      <c r="G59" s="2" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>113955</v>
+      </c>
+      <c r="C60" s="2" t="n">
+        <v>0.1333</v>
+      </c>
+      <c r="D60" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="G60" s="2"/>
+      <c r="E60" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F60" s="0" t="n">
+        <v>113968</v>
+      </c>
+      <c r="G60" s="2" t="n">
+        <v>0.1333</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="3" t="n">
         <f aca="false">SUM(B47:B60)</f>
-        <v>766763</v>
+        <v>1230289</v>
       </c>
       <c r="C61" s="4" t="n">
         <f aca="false">AVERAGE(C47:C60)</f>
-        <v>0.914811111111111</v>
+        <v>0.819035714285714</v>
       </c>
       <c r="D61" s="3" t="n">
         <f aca="false">SUM(D47:D60)</f>
-        <v>0</v>
-      </c>
-      <c r="E61" s="4" t="e">
+        <v>7084395</v>
+      </c>
+      <c r="E61" s="4" t="n">
         <f aca="false">AVERAGE(E47:E60)</f>
-        <v>#DIV/0!</v>
+        <v>0.997438461538462</v>
       </c>
       <c r="F61" s="3" t="n">
         <f aca="false">SUM(F47:F60)</f>
-        <v>0</v>
-      </c>
-      <c r="G61" s="4" t="e">
+        <v>1232043</v>
+      </c>
+      <c r="G61" s="4" t="n">
         <f aca="false">AVERAGE(G47:G60)</f>
-        <v>#DIV/0!</v>
+        <v>0.821421428571429</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1363,6 +1525,309 @@
         <v>26</v>
       </c>
       <c r="B66" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B69" s="0" t="n">
+        <v>68018</v>
+      </c>
+      <c r="C69" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D69" s="0" t="n">
+        <v>69280</v>
+      </c>
+      <c r="E69" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G69" s="2"/>
+    </row>
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B70" s="0" t="n">
+        <v>95306</v>
+      </c>
+      <c r="C70" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <v>119521</v>
+      </c>
+      <c r="E70" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G70" s="2"/>
+    </row>
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B71" s="0" t="n">
+        <v>88207</v>
+      </c>
+      <c r="C71" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D71" s="0" t="n">
+        <v>161192</v>
+      </c>
+      <c r="E71" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G71" s="2"/>
+    </row>
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B72" s="0" t="n">
+        <v>80090</v>
+      </c>
+      <c r="C72" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D72" s="0" t="n">
+        <v>259379</v>
+      </c>
+      <c r="E72" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G72" s="2"/>
+    </row>
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B73" s="0" t="n">
+        <v>89513</v>
+      </c>
+      <c r="C73" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D73" s="0" t="n">
+        <v>237880</v>
+      </c>
+      <c r="E73" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G73" s="2"/>
+    </row>
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B74" s="0" t="n">
+        <v>78731</v>
+      </c>
+      <c r="C74" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G74" s="2"/>
+    </row>
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B75" s="0" t="n">
+        <v>77748</v>
+      </c>
+      <c r="C75" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E75" s="2"/>
+      <c r="G75" s="2"/>
+    </row>
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B76" s="0" t="n">
+        <v>79517</v>
+      </c>
+      <c r="C76" s="2" t="n">
+        <v>0.6667</v>
+      </c>
+      <c r="E76" s="2"/>
+      <c r="G76" s="2"/>
+    </row>
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B77" s="0" t="n">
+        <v>84620</v>
+      </c>
+      <c r="C77" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E77" s="2"/>
+      <c r="G77" s="2"/>
+    </row>
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B78" s="0" t="n">
+        <v>93645</v>
+      </c>
+      <c r="C78" s="2" t="n">
+        <v>0.9333</v>
+      </c>
+      <c r="E78" s="2"/>
+      <c r="G78" s="2"/>
+    </row>
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B79" s="0" t="n">
+        <v>92876</v>
+      </c>
+      <c r="C79" s="2" t="n">
+        <v>0.9333</v>
+      </c>
+      <c r="E79" s="2"/>
+      <c r="G79" s="2"/>
+    </row>
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B80" s="0" t="n">
+        <v>103613</v>
+      </c>
+      <c r="C80" s="2" t="n">
+        <v>0.3333</v>
+      </c>
+      <c r="E80" s="2"/>
+      <c r="G80" s="2"/>
+    </row>
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B81" s="0" t="n">
+        <v>50228</v>
+      </c>
+      <c r="C81" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E81" s="2"/>
+      <c r="G81" s="2"/>
+    </row>
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B82" s="0" t="n">
+        <v>113955</v>
+      </c>
+      <c r="C82" s="2" t="n">
+        <v>0.1333</v>
+      </c>
+      <c r="D82" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G82" s="2"/>
+    </row>
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="3" t="n">
+        <f aca="false">SUM(B69:B82)</f>
+        <v>1196067</v>
+      </c>
+      <c r="C83" s="4" t="n">
+        <f aca="false">AVERAGE(C69:C82)</f>
+        <v>0.821421428571429</v>
+      </c>
+      <c r="D83" s="3" t="n">
+        <f aca="false">SUM(D69:D82)</f>
+        <v>847252</v>
+      </c>
+      <c r="E83" s="4" t="n">
+        <f aca="false">AVERAGE(E69:E82)</f>
+        <v>1</v>
+      </c>
+      <c r="F83" s="3" t="n">
+        <f aca="false">SUM(F69:F82)</f>
+        <v>0</v>
+      </c>
+      <c r="G83" s="4" t="e">
+        <f aca="false">AVERAGE(G69:G82)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B84" s="6" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B85" s="6" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B88" s="0" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1385,7 +1850,7 @@
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F38" activeCellId="0" sqref="F38"/>
+      <selection pane="topLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>